<commit_message>
updates following the addition of randomization to study
</commit_message>
<xml_diff>
--- a/data/p1_rm.xlsx
+++ b/data/p1_rm.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimwright/Desktop/University of Oregon Courses/Dissertation/Proposal /"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimwright/Desktop/University of Oregon Courses/Dissertation/Proposal /proposal_measures/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{807E1FBB-9397-2342-9A41-B1291E115D08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28B037DA-CE4B-EC49-8F23-8BDB7F04E8BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="720" yWindow="940" windowWidth="27640" windowHeight="15760" xr2:uid="{B02A89B2-23A3-1B47-8154-275295DF617A}"/>
   </bookViews>
@@ -393,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25A523DB-5BF0-D542-895B-921F2D2E9D40}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B5" sqref="B5:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -414,89 +414,34 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C3">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5">
-        <v>9</v>
-      </c>
-      <c r="B5">
-        <v>5</v>
-      </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6">
-        <v>10</v>
-      </c>
-      <c r="B6">
-        <v>4</v>
-      </c>
-      <c r="C6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7">
-        <v>11</v>
-      </c>
-      <c r="B7">
-        <v>4</v>
-      </c>
-      <c r="C7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8">
-        <v>12</v>
-      </c>
-      <c r="B8">
-        <v>5</v>
-      </c>
-      <c r="C8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9">
-        <v>13</v>
-      </c>
-      <c r="B9">
-        <v>5</v>
-      </c>
-      <c r="C9">
         <v>4</v>
       </c>
     </row>

</xml_diff>